<commit_message>
changed pipeline order and made all steps more dynamic and generalizable to other SeqTrial data setups
</commit_message>
<xml_diff>
--- a/DataSetup/data-setup_intervals_eld.xlsx
+++ b/DataSetup/data-setup_intervals_eld.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/switchdrive/Alain/PostDoc_DKF/TTE_metfin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/Documents/GitHub/metformin_covid/DataSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ADCAAA-3D9E-EF49-90FA-21BE905723CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B5C02F-7736-FB4A-9C45-48AC7D3489A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{D2626234-9DAF-A64C-B48A-88D45276679D}"/>
+    <workbookView xWindow="680" yWindow="860" windowWidth="28040" windowHeight="17260" xr2:uid="{D2626234-9DAF-A64C-B48A-88D45276679D}"/>
   </bookViews>
   <sheets>
     <sheet name="df_main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="45">
   <si>
     <t>patient_id</t>
   </si>
@@ -139,9 +139,6 @@
     <t>What if HbA1c measurement in same month as death? Death is "shifted up" to previous interval - but what to do with HbA1c? And there might already be a HbA1c measurement in the previous interval!</t>
   </si>
   <si>
-    <t>General rule (also think of scenario where outcome is something else than death): Ignore (time-updated) covariate info in same interval as outcome occurs!</t>
-  </si>
-  <si>
     <t>Note: this is how the dataset looks like before removing the helper rows/variables</t>
   </si>
   <si>
@@ -149,6 +146,33 @@
   </si>
   <si>
     <t>cens_date_dereg</t>
+  </si>
+  <si>
+    <t>General rule (also think of scenario where outcome is something else than death): Ignore (time-updated) covariate info in same interval as outcome occurs! =&gt; by adding ELD first, then shifting up the outcome/comp/censor events and ignoring the row when these events happened, this is automatically taken care of.</t>
+  </si>
+  <si>
+    <t>elig</t>
+  </si>
+  <si>
+    <t>treat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elig: </t>
+  </si>
+  <si>
+    <t>treat:</t>
+  </si>
+  <si>
+    <t>metformin start during interval =&gt; assign 1 to current or next interval?</t>
+  </si>
+  <si>
+    <t>for exclusion criteria such as "prior history of…": what happens during interval, e.g. metformin allergy or liver disease =&gt; exclusion from next interval onwards (using lagged info)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">however, for exclusion criteria "no prior treatment with other antidiabetic" we might want to be "stricter" to uphold comparison metformin vs nothing, and exclude people not only if other antidiabetic treatment in prior but also in current interval? </t>
+  </si>
+  <si>
+    <t>same question for very high HbA1c exclusion criteria</t>
   </si>
 </sst>
 </file>
@@ -619,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CD69BF-2E2C-364E-B7C6-5886BE0B7FC9}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +666,7 @@
     <col min="13" max="13" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,10 +677,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>28</v>
@@ -682,8 +706,14 @@
       <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -724,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -765,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -806,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -847,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -888,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -929,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -970,7 +1000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -1011,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -1052,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>3</v>
       </c>
@@ -1093,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>4</v>
       </c>
@@ -1134,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -1175,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>4</v>
       </c>
@@ -1214,6 +1244,35 @@
       </c>
       <c r="M14" s="16">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1285,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1419,7 @@
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2326,7 +2385,7 @@
     </row>
     <row r="18" spans="1:16" s="22" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
align dummy data size
</commit_message>
<xml_diff>
--- a/DataSetup/data-setup_intervals_eld.xlsx
+++ b/DataSetup/data-setup_intervals_eld.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/Documents/GitHub/metformin_covid/DataSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B5C02F-7736-FB4A-9C45-48AC7D3489A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4782E1-2F2C-AD43-BA21-02943575025E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="860" windowWidth="28040" windowHeight="17260" xr2:uid="{D2626234-9DAF-A64C-B48A-88D45276679D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="45">
   <si>
     <t>patient_id</t>
   </si>
@@ -163,23 +163,83 @@
     <t>treat:</t>
   </si>
   <si>
-    <t>metformin start during interval =&gt; assign 1 to current or next interval?</t>
-  </si>
-  <si>
-    <t>for exclusion criteria such as "prior history of…": what happens during interval, e.g. metformin allergy or liver disease =&gt; exclusion from next interval onwards (using lagged info)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">however, for exclusion criteria "no prior treatment with other antidiabetic" we might want to be "stricter" to uphold comparison metformin vs nothing, and exclude people not only if other antidiabetic treatment in prior but also in current interval? </t>
-  </si>
-  <si>
-    <t>same question for very high HbA1c exclusion criteria</t>
+    <t>baseline_date</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">metformin start during interval =&gt; assign 1 to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>current</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or next interval?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"no prior treatment with other antidiabetic" =&gt; exclusion from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>current</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interval onwards (to make sure someone is ineligible who started metformin and another antidiabetic in same month)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"prior history of..." (liver disease, metformin allergy, any covid event) =&gt; exclusion from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>next</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interval onwards (using lagged info)?</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +267,11 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -643,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CD69BF-2E2C-364E-B7C6-5886BE0B7FC9}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +720,7 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -671,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -843,7 +908,7 @@
       <c r="B5" s="3">
         <v>43861</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="19">
         <v>44007</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -858,16 +923,16 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="20">
         <v>43952</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="20">
         <v>43981</v>
       </c>
       <c r="J5" s="2">
         <v>3</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="18">
         <v>1</v>
       </c>
       <c r="L5" s="5">
@@ -891,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="9">
-        <v>43900</v>
+        <v>43931</v>
       </c>
       <c r="F6" s="8">
         <v>60</v>
@@ -932,7 +997,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="9">
-        <v>43900</v>
+        <v>43931</v>
       </c>
       <c r="F7" s="8">
         <v>60</v>
@@ -973,7 +1038,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="9">
-        <v>43900</v>
+        <v>43931</v>
       </c>
       <c r="F8" s="8">
         <v>60</v>
@@ -1011,7 +1076,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="13">
-        <v>43905</v>
+        <v>43936</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>12</v>
@@ -1052,7 +1117,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="13">
-        <v>43905</v>
+        <v>43936</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>12</v>
@@ -1093,7 +1158,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="13">
-        <v>43905</v>
+        <v>43936</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>12</v>
@@ -1251,7 +1316,7 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,20 +1324,12 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
       <c r="B19" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporated eligibility criteria: "any incident T2DM diagnosis within prior 6 months"
</commit_message>
<xml_diff>
--- a/DataSetup/data-setup_intervals_eld.xlsx
+++ b/DataSetup/data-setup_intervals_eld.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amstutzal/Documents/GitHub/metformin_covid/DataSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4782E1-2F2C-AD43-BA21-02943575025E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010A7078-CF95-3B4D-AF9C-A9AB0273335D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="860" windowWidth="28040" windowHeight="17260" xr2:uid="{D2626234-9DAF-A64C-B48A-88D45276679D}"/>
+    <workbookView xWindow="680" yWindow="840" windowWidth="28040" windowHeight="17260" xr2:uid="{D2626234-9DAF-A64C-B48A-88D45276679D}"/>
   </bookViews>
   <sheets>
     <sheet name="df_main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="47">
   <si>
     <t>patient_id</t>
   </si>
@@ -164,29 +164,6 @@
   </si>
   <si>
     <t>baseline_date</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">metformin start during interval =&gt; assign 1 to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>current</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or next interval?</t>
-    </r>
   </si>
   <si>
     <r>
@@ -213,6 +190,32 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">metformin start during interval =&gt; assign 1 to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>current</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interval! Yes!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">outcomes: </t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">"prior history of..." (liver disease, metformin allergy, any covid event) =&gt; exclusion from </t>
     </r>
     <r>
@@ -231,8 +234,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> interval onwards (using lagged info)?</t>
+      <t xml:space="preserve"> interval onwards (using lagged info)! -&gt; YES, because you don't want to exclude someone based on future info during that interval, i.e. at the start of interval you don't know yet if excluded or not, so keep, one only knows in next interval. We "shift the exclusion info to the start of the interval" (the next one)</t>
     </r>
+  </si>
+  <si>
+    <t>shift up 1 interval to avoid that something can happen after the outcome, esp. being treated after the outcome! We shift the outcome info to "the end of the interval" (of the previous). It is not a problem with an outcome such as death, where nothing can happen afterwards, this we would not have to shift, but the other outcomes we do better shift, to ensure correct order between treatment and outcome.</t>
   </si>
 </sst>
 </file>
@@ -708,15 +714,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CD69BF-2E2C-364E-B7C6-5886BE0B7FC9}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1311,25 +1317,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>